<commit_message>
merubah konfigurasi import data absensi
</commit_message>
<xml_diff>
--- a/tests/2022 - 07 - Attendance Details.xlsx
+++ b/tests/2022 - 07 - Attendance Details.xlsx
@@ -39,13 +39,13 @@
     <t>Person ID</t>
   </si>
   <si>
-    <t>Nur A</t>
-  </si>
-  <si>
     <t>Approve 01</t>
   </si>
   <si>
     <t>User 01</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -856,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A282" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J297" sqref="J297"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,7 +891,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1">
         <v>44713</v>
@@ -908,7 +908,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
         <v>44714</v>
@@ -925,7 +925,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1">
         <v>44715</v>
@@ -942,7 +942,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
         <v>44716</v>
@@ -959,7 +959,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1">
         <v>44717</v>
@@ -976,7 +976,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1">
         <v>44718</v>
@@ -993,7 +993,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1">
         <v>44719</v>
@@ -1010,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
         <v>44720</v>
@@ -1027,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1">
         <v>44721</v>
@@ -1044,7 +1044,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1">
         <v>44722</v>
@@ -1061,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1">
         <v>44723</v>
@@ -1078,7 +1078,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1">
         <v>44724</v>
@@ -1095,7 +1095,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1">
         <v>44725</v>
@@ -1112,7 +1112,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1">
         <v>44726</v>
@@ -1129,7 +1129,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C16" s="1">
         <v>44727</v>
@@ -1146,7 +1146,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C17" s="1">
         <v>44728</v>
@@ -1163,7 +1163,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C18" s="1">
         <v>44729</v>
@@ -1180,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C19" s="1">
         <v>44730</v>
@@ -1197,7 +1197,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1">
         <v>44731</v>
@@ -1214,7 +1214,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C21" s="1">
         <v>44732</v>
@@ -1231,7 +1231,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C22" s="1">
         <v>44733</v>
@@ -1248,7 +1248,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C23" s="1">
         <v>44734</v>
@@ -1265,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C24" s="1">
         <v>44735</v>
@@ -1282,7 +1282,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C25" s="1">
         <v>44736</v>
@@ -1299,7 +1299,7 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C26" s="1">
         <v>44737</v>
@@ -1316,7 +1316,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C27" s="1">
         <v>44738</v>
@@ -1333,7 +1333,7 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C28" s="1">
         <v>44739</v>
@@ -1350,7 +1350,7 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C29" s="1">
         <v>44740</v>
@@ -1367,7 +1367,7 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C30" s="1">
         <v>44741</v>
@@ -1384,7 +1384,7 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C31" s="1">
         <v>44742</v>
@@ -1401,7 +1401,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C32" s="1">
         <v>44743</v>
@@ -1418,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C33" s="1">
         <v>44744</v>
@@ -1435,7 +1435,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C34" s="1">
         <v>44745</v>
@@ -1452,7 +1452,7 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C35" s="1">
         <v>44746</v>
@@ -1469,7 +1469,7 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C36" s="1">
         <v>44747</v>
@@ -1486,7 +1486,7 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C37" s="1">
         <v>44748</v>
@@ -1503,7 +1503,7 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C38" s="1">
         <v>44749</v>
@@ -1520,7 +1520,7 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C39" s="1">
         <v>44750</v>
@@ -1537,7 +1537,7 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C40" s="1">
         <v>44751</v>
@@ -1554,7 +1554,7 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C41" s="1">
         <v>44752</v>
@@ -1571,7 +1571,7 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C42" s="1">
         <v>44753</v>
@@ -1588,7 +1588,7 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C43" s="1">
         <v>44754</v>
@@ -1605,7 +1605,7 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C44" s="1">
         <v>44755</v>
@@ -1622,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C45" s="1">
         <v>44756</v>
@@ -1639,7 +1639,7 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C46" s="1">
         <v>44757</v>
@@ -1656,7 +1656,7 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C47" s="1">
         <v>44758</v>
@@ -1673,7 +1673,7 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C48" s="1">
         <v>44759</v>
@@ -1690,7 +1690,7 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C49" s="1">
         <v>44760</v>
@@ -1707,7 +1707,7 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C50" s="1">
         <v>44761</v>
@@ -1724,7 +1724,7 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C51" s="1">
         <v>44762</v>
@@ -1741,7 +1741,7 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C52" s="1">
         <v>44763</v>
@@ -1758,7 +1758,7 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C53" s="1">
         <v>44764</v>
@@ -1775,7 +1775,7 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C54" s="1">
         <v>44765</v>
@@ -1792,7 +1792,7 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C55" s="1">
         <v>44766</v>
@@ -1809,7 +1809,7 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C56" s="1">
         <v>44767</v>
@@ -1826,7 +1826,7 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C57" s="1">
         <v>44768</v>
@@ -1843,7 +1843,7 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C58" s="1">
         <v>44769</v>
@@ -1860,7 +1860,7 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C59" s="1">
         <v>44770</v>
@@ -1877,7 +1877,7 @@
         <v>1</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C60" s="1">
         <v>44771</v>
@@ -1894,7 +1894,7 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C61" s="1">
         <v>44772</v>
@@ -1911,7 +1911,7 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C62" s="1">
         <v>44773</v>
@@ -1928,7 +1928,7 @@
         <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C63" s="1">
         <v>44774</v>
@@ -1945,7 +1945,7 @@
         <v>1</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C64" s="1">
         <v>44775</v>
@@ -1962,7 +1962,7 @@
         <v>1</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C65" s="1">
         <v>44776</v>
@@ -1979,7 +1979,7 @@
         <v>1</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C66" s="1">
         <v>44777</v>
@@ -1996,7 +1996,7 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C67" s="1">
         <v>44778</v>
@@ -2013,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C68" s="1">
         <v>44779</v>
@@ -2030,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C69" s="1">
         <v>44780</v>
@@ -2047,7 +2047,7 @@
         <v>1</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C70" s="1">
         <v>44781</v>
@@ -2064,7 +2064,7 @@
         <v>1</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C71" s="1">
         <v>44782</v>
@@ -2081,7 +2081,7 @@
         <v>1</v>
       </c>
       <c r="B72" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C72" s="1">
         <v>44783</v>
@@ -2098,7 +2098,7 @@
         <v>1</v>
       </c>
       <c r="B73" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C73" s="1">
         <v>44784</v>
@@ -2115,7 +2115,7 @@
         <v>1</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C74" s="1">
         <v>44785</v>
@@ -2132,7 +2132,7 @@
         <v>1</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C75" s="1">
         <v>44786</v>
@@ -2149,7 +2149,7 @@
         <v>1</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C76" s="1">
         <v>44787</v>
@@ -2166,7 +2166,7 @@
         <v>1</v>
       </c>
       <c r="B77" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C77" s="1">
         <v>44788</v>
@@ -2183,7 +2183,7 @@
         <v>1</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C78" s="1">
         <v>44789</v>
@@ -2200,7 +2200,7 @@
         <v>1</v>
       </c>
       <c r="B79" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C79" s="1">
         <v>44790</v>
@@ -2217,7 +2217,7 @@
         <v>1</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C80" s="1">
         <v>44791</v>
@@ -2234,7 +2234,7 @@
         <v>1</v>
       </c>
       <c r="B81" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C81" s="1">
         <v>44792</v>
@@ -2251,7 +2251,7 @@
         <v>1</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C82" s="1">
         <v>44793</v>
@@ -2268,7 +2268,7 @@
         <v>1</v>
       </c>
       <c r="B83" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C83" s="1">
         <v>44794</v>
@@ -2285,7 +2285,7 @@
         <v>1</v>
       </c>
       <c r="B84" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C84" s="1">
         <v>44795</v>
@@ -2302,7 +2302,7 @@
         <v>1</v>
       </c>
       <c r="B85" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C85" s="1">
         <v>44796</v>
@@ -2319,7 +2319,7 @@
         <v>1</v>
       </c>
       <c r="B86" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C86" s="1">
         <v>44797</v>
@@ -2336,7 +2336,7 @@
         <v>1</v>
       </c>
       <c r="B87" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C87" s="1">
         <v>44798</v>
@@ -2353,7 +2353,7 @@
         <v>1</v>
       </c>
       <c r="B88" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C88" s="1">
         <v>44799</v>
@@ -2370,7 +2370,7 @@
         <v>1</v>
       </c>
       <c r="B89" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C89" s="1">
         <v>44800</v>
@@ -2387,7 +2387,7 @@
         <v>1</v>
       </c>
       <c r="B90" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C90" s="1">
         <v>44801</v>
@@ -2404,7 +2404,7 @@
         <v>1</v>
       </c>
       <c r="B91" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C91" s="1">
         <v>44802</v>
@@ -2421,7 +2421,7 @@
         <v>1</v>
       </c>
       <c r="B92" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C92" s="1">
         <v>44803</v>
@@ -2438,7 +2438,7 @@
         <v>1</v>
       </c>
       <c r="B93" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C93" s="1">
         <v>44804</v>
@@ -2455,7 +2455,7 @@
         <v>1</v>
       </c>
       <c r="B94" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C94" s="1">
         <v>44805</v>
@@ -2472,7 +2472,7 @@
         <v>1</v>
       </c>
       <c r="B95" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C95" s="1">
         <v>44806</v>
@@ -2489,7 +2489,7 @@
         <v>1</v>
       </c>
       <c r="B96" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C96" s="1">
         <v>44807</v>
@@ -2506,7 +2506,7 @@
         <v>1</v>
       </c>
       <c r="B97" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C97" s="1">
         <v>44808</v>
@@ -2523,7 +2523,7 @@
         <v>1</v>
       </c>
       <c r="B98" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C98" s="1">
         <v>44809</v>
@@ -2540,7 +2540,7 @@
         <v>1</v>
       </c>
       <c r="B99" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C99" s="1">
         <v>44810</v>
@@ -2557,7 +2557,7 @@
         <v>1</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C100" s="1">
         <v>44811</v>
@@ -2574,7 +2574,7 @@
         <v>1</v>
       </c>
       <c r="B101" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C101" s="1">
         <v>44812</v>
@@ -2591,7 +2591,7 @@
         <v>2</v>
       </c>
       <c r="B102" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C102" s="1">
         <v>44713</v>
@@ -2608,7 +2608,7 @@
         <v>2</v>
       </c>
       <c r="B103" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C103" s="1">
         <v>44714</v>
@@ -2625,7 +2625,7 @@
         <v>2</v>
       </c>
       <c r="B104" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C104" s="1">
         <v>44715</v>
@@ -2642,7 +2642,7 @@
         <v>2</v>
       </c>
       <c r="B105" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C105" s="1">
         <v>44716</v>
@@ -2659,7 +2659,7 @@
         <v>2</v>
       </c>
       <c r="B106" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C106" s="1">
         <v>44717</v>
@@ -2676,7 +2676,7 @@
         <v>2</v>
       </c>
       <c r="B107" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C107" s="1">
         <v>44718</v>
@@ -2693,7 +2693,7 @@
         <v>2</v>
       </c>
       <c r="B108" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C108" s="1">
         <v>44719</v>
@@ -2710,7 +2710,7 @@
         <v>2</v>
       </c>
       <c r="B109" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C109" s="1">
         <v>44720</v>
@@ -2727,7 +2727,7 @@
         <v>2</v>
       </c>
       <c r="B110" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C110" s="1">
         <v>44721</v>
@@ -2744,7 +2744,7 @@
         <v>2</v>
       </c>
       <c r="B111" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C111" s="1">
         <v>44722</v>
@@ -2761,7 +2761,7 @@
         <v>2</v>
       </c>
       <c r="B112" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C112" s="1">
         <v>44723</v>
@@ -2778,7 +2778,7 @@
         <v>2</v>
       </c>
       <c r="B113" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C113" s="1">
         <v>44724</v>
@@ -2795,7 +2795,7 @@
         <v>2</v>
       </c>
       <c r="B114" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C114" s="1">
         <v>44725</v>
@@ -2812,7 +2812,7 @@
         <v>2</v>
       </c>
       <c r="B115" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C115" s="1">
         <v>44726</v>
@@ -2829,7 +2829,7 @@
         <v>2</v>
       </c>
       <c r="B116" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C116" s="1">
         <v>44727</v>
@@ -2846,7 +2846,7 @@
         <v>2</v>
       </c>
       <c r="B117" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C117" s="1">
         <v>44728</v>
@@ -2863,7 +2863,7 @@
         <v>2</v>
       </c>
       <c r="B118" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C118" s="1">
         <v>44729</v>
@@ -2880,7 +2880,7 @@
         <v>2</v>
       </c>
       <c r="B119" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C119" s="1">
         <v>44730</v>
@@ -2897,7 +2897,7 @@
         <v>2</v>
       </c>
       <c r="B120" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C120" s="1">
         <v>44731</v>
@@ -2914,7 +2914,7 @@
         <v>2</v>
       </c>
       <c r="B121" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C121" s="1">
         <v>44732</v>
@@ -2931,7 +2931,7 @@
         <v>2</v>
       </c>
       <c r="B122" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C122" s="1">
         <v>44733</v>
@@ -2948,7 +2948,7 @@
         <v>2</v>
       </c>
       <c r="B123" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C123" s="1">
         <v>44734</v>
@@ -2965,7 +2965,7 @@
         <v>2</v>
       </c>
       <c r="B124" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C124" s="1">
         <v>44735</v>
@@ -2982,7 +2982,7 @@
         <v>2</v>
       </c>
       <c r="B125" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C125" s="1">
         <v>44736</v>
@@ -2999,7 +2999,7 @@
         <v>2</v>
       </c>
       <c r="B126" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C126" s="1">
         <v>44737</v>
@@ -3016,7 +3016,7 @@
         <v>2</v>
       </c>
       <c r="B127" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C127" s="1">
         <v>44738</v>
@@ -3033,7 +3033,7 @@
         <v>2</v>
       </c>
       <c r="B128" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C128" s="1">
         <v>44739</v>
@@ -3050,7 +3050,7 @@
         <v>2</v>
       </c>
       <c r="B129" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C129" s="1">
         <v>44740</v>
@@ -3067,7 +3067,7 @@
         <v>2</v>
       </c>
       <c r="B130" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C130" s="1">
         <v>44741</v>
@@ -3084,7 +3084,7 @@
         <v>2</v>
       </c>
       <c r="B131" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C131" s="1">
         <v>44742</v>
@@ -3101,7 +3101,7 @@
         <v>2</v>
       </c>
       <c r="B132" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C132" s="1">
         <v>44743</v>
@@ -3118,7 +3118,7 @@
         <v>2</v>
       </c>
       <c r="B133" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C133" s="1">
         <v>44744</v>
@@ -3135,7 +3135,7 @@
         <v>2</v>
       </c>
       <c r="B134" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C134" s="1">
         <v>44745</v>
@@ -3152,7 +3152,7 @@
         <v>2</v>
       </c>
       <c r="B135" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C135" s="1">
         <v>44746</v>
@@ -3169,7 +3169,7 @@
         <v>2</v>
       </c>
       <c r="B136" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C136" s="1">
         <v>44747</v>
@@ -3186,7 +3186,7 @@
         <v>2</v>
       </c>
       <c r="B137" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C137" s="1">
         <v>44748</v>
@@ -3203,7 +3203,7 @@
         <v>2</v>
       </c>
       <c r="B138" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C138" s="1">
         <v>44749</v>
@@ -3220,7 +3220,7 @@
         <v>2</v>
       </c>
       <c r="B139" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C139" s="1">
         <v>44750</v>
@@ -3237,7 +3237,7 @@
         <v>2</v>
       </c>
       <c r="B140" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C140" s="1">
         <v>44751</v>
@@ -3254,7 +3254,7 @@
         <v>2</v>
       </c>
       <c r="B141" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C141" s="1">
         <v>44752</v>
@@ -3271,7 +3271,7 @@
         <v>2</v>
       </c>
       <c r="B142" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C142" s="1">
         <v>44753</v>
@@ -3288,7 +3288,7 @@
         <v>2</v>
       </c>
       <c r="B143" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C143" s="1">
         <v>44754</v>
@@ -3305,7 +3305,7 @@
         <v>2</v>
       </c>
       <c r="B144" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C144" s="1">
         <v>44755</v>
@@ -3322,7 +3322,7 @@
         <v>2</v>
       </c>
       <c r="B145" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C145" s="1">
         <v>44756</v>
@@ -3339,7 +3339,7 @@
         <v>2</v>
       </c>
       <c r="B146" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C146" s="1">
         <v>44757</v>
@@ -3356,7 +3356,7 @@
         <v>2</v>
       </c>
       <c r="B147" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C147" s="1">
         <v>44758</v>
@@ -3373,7 +3373,7 @@
         <v>2</v>
       </c>
       <c r="B148" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C148" s="1">
         <v>44759</v>
@@ -3390,7 +3390,7 @@
         <v>2</v>
       </c>
       <c r="B149" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C149" s="1">
         <v>44760</v>
@@ -3407,7 +3407,7 @@
         <v>2</v>
       </c>
       <c r="B150" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C150" s="1">
         <v>44761</v>
@@ -3424,7 +3424,7 @@
         <v>2</v>
       </c>
       <c r="B151" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C151" s="1">
         <v>44762</v>
@@ -3441,7 +3441,7 @@
         <v>2</v>
       </c>
       <c r="B152" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C152" s="1">
         <v>44763</v>
@@ -3458,7 +3458,7 @@
         <v>2</v>
       </c>
       <c r="B153" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C153" s="1">
         <v>44764</v>
@@ -3475,7 +3475,7 @@
         <v>2</v>
       </c>
       <c r="B154" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C154" s="1">
         <v>44765</v>
@@ -3492,7 +3492,7 @@
         <v>2</v>
       </c>
       <c r="B155" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C155" s="1">
         <v>44766</v>
@@ -3509,7 +3509,7 @@
         <v>2</v>
       </c>
       <c r="B156" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C156" s="1">
         <v>44767</v>
@@ -3526,7 +3526,7 @@
         <v>2</v>
       </c>
       <c r="B157" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C157" s="1">
         <v>44768</v>
@@ -3543,7 +3543,7 @@
         <v>2</v>
       </c>
       <c r="B158" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C158" s="1">
         <v>44769</v>
@@ -3560,7 +3560,7 @@
         <v>2</v>
       </c>
       <c r="B159" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C159" s="1">
         <v>44770</v>
@@ -3577,7 +3577,7 @@
         <v>2</v>
       </c>
       <c r="B160" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C160" s="1">
         <v>44771</v>
@@ -3594,7 +3594,7 @@
         <v>2</v>
       </c>
       <c r="B161" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C161" s="1">
         <v>44772</v>
@@ -3611,7 +3611,7 @@
         <v>2</v>
       </c>
       <c r="B162" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C162" s="1">
         <v>44773</v>
@@ -3628,7 +3628,7 @@
         <v>2</v>
       </c>
       <c r="B163" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C163" s="1">
         <v>44774</v>
@@ -3645,7 +3645,7 @@
         <v>2</v>
       </c>
       <c r="B164" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C164" s="1">
         <v>44775</v>
@@ -3662,7 +3662,7 @@
         <v>2</v>
       </c>
       <c r="B165" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C165" s="1">
         <v>44776</v>
@@ -3679,7 +3679,7 @@
         <v>2</v>
       </c>
       <c r="B166" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C166" s="1">
         <v>44777</v>
@@ -3696,7 +3696,7 @@
         <v>2</v>
       </c>
       <c r="B167" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C167" s="1">
         <v>44778</v>
@@ -3713,7 +3713,7 @@
         <v>2</v>
       </c>
       <c r="B168" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C168" s="1">
         <v>44779</v>
@@ -3730,7 +3730,7 @@
         <v>2</v>
       </c>
       <c r="B169" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C169" s="1">
         <v>44780</v>
@@ -3747,7 +3747,7 @@
         <v>2</v>
       </c>
       <c r="B170" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C170" s="1">
         <v>44781</v>
@@ -3764,7 +3764,7 @@
         <v>2</v>
       </c>
       <c r="B171" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C171" s="1">
         <v>44782</v>
@@ -3781,7 +3781,7 @@
         <v>2</v>
       </c>
       <c r="B172" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C172" s="1">
         <v>44783</v>
@@ -3798,7 +3798,7 @@
         <v>2</v>
       </c>
       <c r="B173" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C173" s="1">
         <v>44784</v>
@@ -3815,7 +3815,7 @@
         <v>2</v>
       </c>
       <c r="B174" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C174" s="1">
         <v>44785</v>
@@ -3832,7 +3832,7 @@
         <v>2</v>
       </c>
       <c r="B175" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C175" s="1">
         <v>44786</v>
@@ -3849,7 +3849,7 @@
         <v>2</v>
       </c>
       <c r="B176" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C176" s="1">
         <v>44787</v>
@@ -3866,7 +3866,7 @@
         <v>2</v>
       </c>
       <c r="B177" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C177" s="1">
         <v>44788</v>
@@ -3883,7 +3883,7 @@
         <v>2</v>
       </c>
       <c r="B178" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C178" s="1">
         <v>44789</v>
@@ -3900,7 +3900,7 @@
         <v>2</v>
       </c>
       <c r="B179" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C179" s="1">
         <v>44790</v>
@@ -3917,7 +3917,7 @@
         <v>2</v>
       </c>
       <c r="B180" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C180" s="1">
         <v>44791</v>
@@ -3934,7 +3934,7 @@
         <v>2</v>
       </c>
       <c r="B181" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C181" s="1">
         <v>44792</v>
@@ -3951,7 +3951,7 @@
         <v>2</v>
       </c>
       <c r="B182" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C182" s="1">
         <v>44793</v>
@@ -3968,7 +3968,7 @@
         <v>2</v>
       </c>
       <c r="B183" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C183" s="1">
         <v>44794</v>
@@ -3985,7 +3985,7 @@
         <v>2</v>
       </c>
       <c r="B184" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C184" s="1">
         <v>44795</v>
@@ -4002,7 +4002,7 @@
         <v>2</v>
       </c>
       <c r="B185" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C185" s="1">
         <v>44796</v>
@@ -4019,7 +4019,7 @@
         <v>2</v>
       </c>
       <c r="B186" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C186" s="1">
         <v>44797</v>
@@ -4036,7 +4036,7 @@
         <v>2</v>
       </c>
       <c r="B187" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C187" s="1">
         <v>44798</v>
@@ -4053,7 +4053,7 @@
         <v>2</v>
       </c>
       <c r="B188" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C188" s="1">
         <v>44799</v>
@@ -4070,7 +4070,7 @@
         <v>2</v>
       </c>
       <c r="B189" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C189" s="1">
         <v>44800</v>
@@ -4087,7 +4087,7 @@
         <v>2</v>
       </c>
       <c r="B190" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C190" s="1">
         <v>44801</v>
@@ -4104,7 +4104,7 @@
         <v>2</v>
       </c>
       <c r="B191" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C191" s="1">
         <v>44802</v>
@@ -4121,7 +4121,7 @@
         <v>2</v>
       </c>
       <c r="B192" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C192" s="1">
         <v>44803</v>
@@ -4138,7 +4138,7 @@
         <v>2</v>
       </c>
       <c r="B193" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C193" s="1">
         <v>44804</v>
@@ -4155,7 +4155,7 @@
         <v>2</v>
       </c>
       <c r="B194" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C194" s="1">
         <v>44805</v>
@@ -4172,7 +4172,7 @@
         <v>2</v>
       </c>
       <c r="B195" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C195" s="1">
         <v>44806</v>
@@ -4189,7 +4189,7 @@
         <v>2</v>
       </c>
       <c r="B196" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C196" s="1">
         <v>44807</v>
@@ -4206,7 +4206,7 @@
         <v>2</v>
       </c>
       <c r="B197" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C197" s="1">
         <v>44808</v>
@@ -4223,7 +4223,7 @@
         <v>2</v>
       </c>
       <c r="B198" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C198" s="1">
         <v>44809</v>
@@ -4240,7 +4240,7 @@
         <v>2</v>
       </c>
       <c r="B199" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C199" s="1">
         <v>44810</v>
@@ -4257,7 +4257,7 @@
         <v>2</v>
       </c>
       <c r="B200" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C200" s="1">
         <v>44811</v>
@@ -4274,7 +4274,7 @@
         <v>2</v>
       </c>
       <c r="B201" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C201" s="1">
         <v>44812</v>
@@ -4291,7 +4291,7 @@
         <v>3</v>
       </c>
       <c r="B202" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C202" s="1">
         <v>44713</v>
@@ -4308,7 +4308,7 @@
         <v>3</v>
       </c>
       <c r="B203" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C203" s="1">
         <v>44714</v>
@@ -4325,7 +4325,7 @@
         <v>3</v>
       </c>
       <c r="B204" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C204" s="1">
         <v>44715</v>
@@ -4342,7 +4342,7 @@
         <v>3</v>
       </c>
       <c r="B205" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C205" s="1">
         <v>44716</v>
@@ -4359,7 +4359,7 @@
         <v>3</v>
       </c>
       <c r="B206" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C206" s="1">
         <v>44717</v>
@@ -4376,7 +4376,7 @@
         <v>3</v>
       </c>
       <c r="B207" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C207" s="1">
         <v>44718</v>
@@ -4393,7 +4393,7 @@
         <v>3</v>
       </c>
       <c r="B208" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C208" s="1">
         <v>44719</v>
@@ -4410,7 +4410,7 @@
         <v>3</v>
       </c>
       <c r="B209" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C209" s="1">
         <v>44720</v>
@@ -4427,7 +4427,7 @@
         <v>3</v>
       </c>
       <c r="B210" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C210" s="1">
         <v>44721</v>
@@ -4444,7 +4444,7 @@
         <v>3</v>
       </c>
       <c r="B211" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C211" s="1">
         <v>44722</v>
@@ -4461,7 +4461,7 @@
         <v>3</v>
       </c>
       <c r="B212" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C212" s="1">
         <v>44723</v>
@@ -4478,7 +4478,7 @@
         <v>3</v>
       </c>
       <c r="B213" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C213" s="1">
         <v>44724</v>
@@ -4495,7 +4495,7 @@
         <v>3</v>
       </c>
       <c r="B214" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C214" s="1">
         <v>44725</v>
@@ -4512,7 +4512,7 @@
         <v>3</v>
       </c>
       <c r="B215" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C215" s="1">
         <v>44726</v>
@@ -4529,7 +4529,7 @@
         <v>3</v>
       </c>
       <c r="B216" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C216" s="1">
         <v>44727</v>
@@ -4546,7 +4546,7 @@
         <v>3</v>
       </c>
       <c r="B217" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C217" s="1">
         <v>44728</v>
@@ -4563,7 +4563,7 @@
         <v>3</v>
       </c>
       <c r="B218" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C218" s="1">
         <v>44729</v>
@@ -4580,7 +4580,7 @@
         <v>3</v>
       </c>
       <c r="B219" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C219" s="1">
         <v>44730</v>
@@ -4597,7 +4597,7 @@
         <v>3</v>
       </c>
       <c r="B220" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C220" s="1">
         <v>44731</v>
@@ -4614,7 +4614,7 @@
         <v>3</v>
       </c>
       <c r="B221" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C221" s="1">
         <v>44732</v>
@@ -4631,7 +4631,7 @@
         <v>3</v>
       </c>
       <c r="B222" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C222" s="1">
         <v>44733</v>
@@ -4648,7 +4648,7 @@
         <v>3</v>
       </c>
       <c r="B223" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C223" s="1">
         <v>44734</v>
@@ -4665,7 +4665,7 @@
         <v>3</v>
       </c>
       <c r="B224" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C224" s="1">
         <v>44735</v>
@@ -4682,7 +4682,7 @@
         <v>3</v>
       </c>
       <c r="B225" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C225" s="1">
         <v>44736</v>
@@ -4699,7 +4699,7 @@
         <v>3</v>
       </c>
       <c r="B226" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C226" s="1">
         <v>44737</v>
@@ -4716,7 +4716,7 @@
         <v>3</v>
       </c>
       <c r="B227" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C227" s="1">
         <v>44738</v>
@@ -4733,7 +4733,7 @@
         <v>3</v>
       </c>
       <c r="B228" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C228" s="1">
         <v>44739</v>
@@ -4750,7 +4750,7 @@
         <v>3</v>
       </c>
       <c r="B229" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C229" s="1">
         <v>44740</v>
@@ -4767,7 +4767,7 @@
         <v>3</v>
       </c>
       <c r="B230" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C230" s="1">
         <v>44741</v>
@@ -4784,7 +4784,7 @@
         <v>3</v>
       </c>
       <c r="B231" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C231" s="1">
         <v>44742</v>
@@ -4801,7 +4801,7 @@
         <v>3</v>
       </c>
       <c r="B232" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C232" s="1">
         <v>44743</v>
@@ -4818,7 +4818,7 @@
         <v>3</v>
       </c>
       <c r="B233" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C233" s="1">
         <v>44744</v>
@@ -4835,7 +4835,7 @@
         <v>3</v>
       </c>
       <c r="B234" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C234" s="1">
         <v>44745</v>
@@ -4852,7 +4852,7 @@
         <v>3</v>
       </c>
       <c r="B235" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C235" s="1">
         <v>44746</v>
@@ -4869,7 +4869,7 @@
         <v>3</v>
       </c>
       <c r="B236" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C236" s="1">
         <v>44747</v>
@@ -4886,7 +4886,7 @@
         <v>3</v>
       </c>
       <c r="B237" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C237" s="1">
         <v>44748</v>
@@ -4903,7 +4903,7 @@
         <v>3</v>
       </c>
       <c r="B238" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C238" s="1">
         <v>44749</v>
@@ -4920,7 +4920,7 @@
         <v>3</v>
       </c>
       <c r="B239" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C239" s="1">
         <v>44750</v>
@@ -4937,7 +4937,7 @@
         <v>3</v>
       </c>
       <c r="B240" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C240" s="1">
         <v>44751</v>
@@ -4954,7 +4954,7 @@
         <v>3</v>
       </c>
       <c r="B241" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C241" s="1">
         <v>44752</v>
@@ -4971,7 +4971,7 @@
         <v>3</v>
       </c>
       <c r="B242" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C242" s="1">
         <v>44753</v>
@@ -4988,7 +4988,7 @@
         <v>3</v>
       </c>
       <c r="B243" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C243" s="1">
         <v>44754</v>
@@ -5005,7 +5005,7 @@
         <v>3</v>
       </c>
       <c r="B244" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C244" s="1">
         <v>44755</v>
@@ -5022,7 +5022,7 @@
         <v>3</v>
       </c>
       <c r="B245" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C245" s="1">
         <v>44756</v>
@@ -5039,7 +5039,7 @@
         <v>3</v>
       </c>
       <c r="B246" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C246" s="1">
         <v>44757</v>
@@ -5056,7 +5056,7 @@
         <v>3</v>
       </c>
       <c r="B247" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C247" s="1">
         <v>44758</v>
@@ -5073,7 +5073,7 @@
         <v>3</v>
       </c>
       <c r="B248" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C248" s="1">
         <v>44759</v>
@@ -5090,7 +5090,7 @@
         <v>3</v>
       </c>
       <c r="B249" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C249" s="1">
         <v>44760</v>
@@ -5107,7 +5107,7 @@
         <v>3</v>
       </c>
       <c r="B250" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C250" s="1">
         <v>44761</v>
@@ -5124,7 +5124,7 @@
         <v>3</v>
       </c>
       <c r="B251" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C251" s="1">
         <v>44762</v>
@@ -5141,7 +5141,7 @@
         <v>3</v>
       </c>
       <c r="B252" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C252" s="1">
         <v>44763</v>
@@ -5158,7 +5158,7 @@
         <v>3</v>
       </c>
       <c r="B253" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C253" s="1">
         <v>44764</v>
@@ -5175,7 +5175,7 @@
         <v>3</v>
       </c>
       <c r="B254" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C254" s="1">
         <v>44765</v>
@@ -5192,7 +5192,7 @@
         <v>3</v>
       </c>
       <c r="B255" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C255" s="1">
         <v>44766</v>
@@ -5209,7 +5209,7 @@
         <v>3</v>
       </c>
       <c r="B256" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C256" s="1">
         <v>44767</v>
@@ -5226,7 +5226,7 @@
         <v>3</v>
       </c>
       <c r="B257" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C257" s="1">
         <v>44768</v>
@@ -5243,7 +5243,7 @@
         <v>3</v>
       </c>
       <c r="B258" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C258" s="1">
         <v>44769</v>
@@ -5260,7 +5260,7 @@
         <v>3</v>
       </c>
       <c r="B259" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C259" s="1">
         <v>44770</v>
@@ -5277,7 +5277,7 @@
         <v>3</v>
       </c>
       <c r="B260" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C260" s="1">
         <v>44771</v>
@@ -5294,7 +5294,7 @@
         <v>3</v>
       </c>
       <c r="B261" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C261" s="1">
         <v>44772</v>
@@ -5311,7 +5311,7 @@
         <v>3</v>
       </c>
       <c r="B262" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C262" s="1">
         <v>44773</v>
@@ -5328,7 +5328,7 @@
         <v>3</v>
       </c>
       <c r="B263" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C263" s="1">
         <v>44774</v>
@@ -5345,7 +5345,7 @@
         <v>3</v>
       </c>
       <c r="B264" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C264" s="1">
         <v>44775</v>
@@ -5362,7 +5362,7 @@
         <v>3</v>
       </c>
       <c r="B265" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C265" s="1">
         <v>44776</v>
@@ -5379,7 +5379,7 @@
         <v>3</v>
       </c>
       <c r="B266" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C266" s="1">
         <v>44777</v>
@@ -5396,7 +5396,7 @@
         <v>3</v>
       </c>
       <c r="B267" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C267" s="1">
         <v>44778</v>
@@ -5413,7 +5413,7 @@
         <v>3</v>
       </c>
       <c r="B268" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C268" s="1">
         <v>44779</v>
@@ -5430,7 +5430,7 @@
         <v>3</v>
       </c>
       <c r="B269" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C269" s="1">
         <v>44780</v>
@@ -5447,7 +5447,7 @@
         <v>3</v>
       </c>
       <c r="B270" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C270" s="1">
         <v>44781</v>
@@ -5464,7 +5464,7 @@
         <v>3</v>
       </c>
       <c r="B271" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C271" s="1">
         <v>44782</v>
@@ -5481,7 +5481,7 @@
         <v>3</v>
       </c>
       <c r="B272" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C272" s="1">
         <v>44783</v>
@@ -5498,7 +5498,7 @@
         <v>3</v>
       </c>
       <c r="B273" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C273" s="1">
         <v>44784</v>
@@ -5515,7 +5515,7 @@
         <v>3</v>
       </c>
       <c r="B274" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C274" s="1">
         <v>44785</v>
@@ -5532,7 +5532,7 @@
         <v>3</v>
       </c>
       <c r="B275" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C275" s="1">
         <v>44786</v>
@@ -5549,7 +5549,7 @@
         <v>3</v>
       </c>
       <c r="B276" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C276" s="1">
         <v>44787</v>
@@ -5566,7 +5566,7 @@
         <v>3</v>
       </c>
       <c r="B277" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C277" s="1">
         <v>44788</v>
@@ -5583,7 +5583,7 @@
         <v>3</v>
       </c>
       <c r="B278" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C278" s="1">
         <v>44789</v>
@@ -5600,7 +5600,7 @@
         <v>3</v>
       </c>
       <c r="B279" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C279" s="1">
         <v>44790</v>
@@ -5617,7 +5617,7 @@
         <v>3</v>
       </c>
       <c r="B280" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C280" s="1">
         <v>44791</v>
@@ -5634,7 +5634,7 @@
         <v>3</v>
       </c>
       <c r="B281" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C281" s="1">
         <v>44792</v>
@@ -5651,7 +5651,7 @@
         <v>3</v>
       </c>
       <c r="B282" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C282" s="1">
         <v>44793</v>
@@ -5668,7 +5668,7 @@
         <v>3</v>
       </c>
       <c r="B283" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C283" s="1">
         <v>44794</v>
@@ -5685,7 +5685,7 @@
         <v>3</v>
       </c>
       <c r="B284" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C284" s="1">
         <v>44795</v>
@@ -5702,7 +5702,7 @@
         <v>3</v>
       </c>
       <c r="B285" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C285" s="1">
         <v>44796</v>
@@ -5719,7 +5719,7 @@
         <v>3</v>
       </c>
       <c r="B286" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C286" s="1">
         <v>44797</v>
@@ -5736,7 +5736,7 @@
         <v>3</v>
       </c>
       <c r="B287" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C287" s="1">
         <v>44798</v>
@@ -5753,7 +5753,7 @@
         <v>3</v>
       </c>
       <c r="B288" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C288" s="1">
         <v>44799</v>
@@ -5770,7 +5770,7 @@
         <v>3</v>
       </c>
       <c r="B289" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C289" s="1">
         <v>44800</v>
@@ -5787,7 +5787,7 @@
         <v>3</v>
       </c>
       <c r="B290" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C290" s="1">
         <v>44801</v>
@@ -5804,7 +5804,7 @@
         <v>3</v>
       </c>
       <c r="B291" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C291" s="1">
         <v>44802</v>
@@ -5821,7 +5821,7 @@
         <v>3</v>
       </c>
       <c r="B292" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C292" s="1">
         <v>44803</v>
@@ -5838,7 +5838,7 @@
         <v>3</v>
       </c>
       <c r="B293" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C293" s="1">
         <v>44804</v>
@@ -5855,7 +5855,7 @@
         <v>3</v>
       </c>
       <c r="B294" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C294" s="1">
         <v>44805</v>
@@ -5872,7 +5872,7 @@
         <v>3</v>
       </c>
       <c r="B295" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C295" s="1">
         <v>44806</v>
@@ -5889,7 +5889,7 @@
         <v>3</v>
       </c>
       <c r="B296" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C296" s="1">
         <v>44807</v>
@@ -5906,7 +5906,7 @@
         <v>3</v>
       </c>
       <c r="B297" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C297" s="1">
         <v>44808</v>
@@ -5923,7 +5923,7 @@
         <v>3</v>
       </c>
       <c r="B298" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C298" s="1">
         <v>44809</v>
@@ -5940,7 +5940,7 @@
         <v>3</v>
       </c>
       <c r="B299" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C299" s="1">
         <v>44810</v>
@@ -5957,7 +5957,7 @@
         <v>3</v>
       </c>
       <c r="B300" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C300" s="1">
         <v>44811</v>
@@ -5974,7 +5974,7 @@
         <v>3</v>
       </c>
       <c r="B301" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C301" s="1">
         <v>44812</v>

</xml_diff>

<commit_message>
memperbaiki fungsi tambah pengajuan setelah dikembalikan dari Approver
</commit_message>
<xml_diff>
--- a/tests/2022 - 07 - Attendance Details.xlsx
+++ b/tests/2022 - 07 - Attendance Details.xlsx
@@ -30,12 +30,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Chek In</t>
-  </si>
-  <si>
-    <t>Chek Out</t>
-  </si>
-  <si>
     <t>Person ID</t>
   </si>
   <si>
@@ -46,6 +40,12 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>Check In</t>
+  </si>
+  <si>
+    <t>Check Out</t>
   </si>
 </sst>
 </file>
@@ -856,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -880,10 +880,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -891,7 +891,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>44713</v>
@@ -908,7 +908,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>44714</v>
@@ -925,7 +925,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>44715</v>
@@ -942,7 +942,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>44716</v>
@@ -959,7 +959,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
         <v>44717</v>
@@ -976,7 +976,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>44718</v>
@@ -993,7 +993,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>44719</v>
@@ -1010,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>44720</v>
@@ -1027,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>44721</v>
@@ -1044,7 +1044,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1">
         <v>44722</v>
@@ -1061,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1">
         <v>44723</v>
@@ -1078,7 +1078,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1">
         <v>44724</v>
@@ -1095,7 +1095,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C14" s="1">
         <v>44725</v>
@@ -1112,7 +1112,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1">
         <v>44726</v>
@@ -1129,7 +1129,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1">
         <v>44727</v>
@@ -1146,7 +1146,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1">
         <v>44728</v>
@@ -1163,7 +1163,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1">
         <v>44729</v>
@@ -1180,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1">
         <v>44730</v>
@@ -1197,7 +1197,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C20" s="1">
         <v>44731</v>
@@ -1214,7 +1214,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C21" s="1">
         <v>44732</v>
@@ -1231,7 +1231,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C22" s="1">
         <v>44733</v>
@@ -1248,7 +1248,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1">
         <v>44734</v>
@@ -1265,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C24" s="1">
         <v>44735</v>
@@ -1282,7 +1282,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C25" s="1">
         <v>44736</v>
@@ -1299,7 +1299,7 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C26" s="1">
         <v>44737</v>
@@ -1316,7 +1316,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C27" s="1">
         <v>44738</v>
@@ -1333,7 +1333,7 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C28" s="1">
         <v>44739</v>
@@ -1350,7 +1350,7 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C29" s="1">
         <v>44740</v>
@@ -1367,7 +1367,7 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C30" s="1">
         <v>44741</v>
@@ -1384,7 +1384,7 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C31" s="1">
         <v>44742</v>
@@ -1401,7 +1401,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C32" s="1">
         <v>44743</v>
@@ -1418,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C33" s="1">
         <v>44744</v>
@@ -1435,7 +1435,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C34" s="1">
         <v>44745</v>
@@ -1452,7 +1452,7 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C35" s="1">
         <v>44746</v>
@@ -1469,7 +1469,7 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C36" s="1">
         <v>44747</v>
@@ -1486,7 +1486,7 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C37" s="1">
         <v>44748</v>
@@ -1503,7 +1503,7 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C38" s="1">
         <v>44749</v>
@@ -1520,7 +1520,7 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C39" s="1">
         <v>44750</v>
@@ -1537,7 +1537,7 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C40" s="1">
         <v>44751</v>
@@ -1554,7 +1554,7 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C41" s="1">
         <v>44752</v>
@@ -1571,7 +1571,7 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C42" s="1">
         <v>44753</v>
@@ -1588,7 +1588,7 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C43" s="1">
         <v>44754</v>
@@ -1605,7 +1605,7 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C44" s="1">
         <v>44755</v>
@@ -1622,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C45" s="1">
         <v>44756</v>
@@ -1639,7 +1639,7 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C46" s="1">
         <v>44757</v>
@@ -1656,7 +1656,7 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C47" s="1">
         <v>44758</v>
@@ -1673,7 +1673,7 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C48" s="1">
         <v>44759</v>
@@ -1690,7 +1690,7 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C49" s="1">
         <v>44760</v>
@@ -1707,7 +1707,7 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C50" s="1">
         <v>44761</v>
@@ -1724,7 +1724,7 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C51" s="1">
         <v>44762</v>
@@ -1741,7 +1741,7 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C52" s="1">
         <v>44763</v>
@@ -1758,7 +1758,7 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C53" s="1">
         <v>44764</v>
@@ -1775,7 +1775,7 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C54" s="1">
         <v>44765</v>
@@ -1792,7 +1792,7 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C55" s="1">
         <v>44766</v>
@@ -1809,7 +1809,7 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C56" s="1">
         <v>44767</v>
@@ -1826,7 +1826,7 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C57" s="1">
         <v>44768</v>
@@ -1843,7 +1843,7 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C58" s="1">
         <v>44769</v>
@@ -1860,7 +1860,7 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C59" s="1">
         <v>44770</v>
@@ -1877,7 +1877,7 @@
         <v>1</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C60" s="1">
         <v>44771</v>
@@ -1894,7 +1894,7 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C61" s="1">
         <v>44772</v>
@@ -1911,7 +1911,7 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C62" s="1">
         <v>44773</v>
@@ -1928,7 +1928,7 @@
         <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C63" s="1">
         <v>44774</v>
@@ -1945,7 +1945,7 @@
         <v>1</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C64" s="1">
         <v>44775</v>
@@ -1962,7 +1962,7 @@
         <v>1</v>
       </c>
       <c r="B65" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C65" s="1">
         <v>44776</v>
@@ -1979,7 +1979,7 @@
         <v>1</v>
       </c>
       <c r="B66" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C66" s="1">
         <v>44777</v>
@@ -1996,7 +1996,7 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C67" s="1">
         <v>44778</v>
@@ -2013,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C68" s="1">
         <v>44779</v>
@@ -2030,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C69" s="1">
         <v>44780</v>
@@ -2047,7 +2047,7 @@
         <v>1</v>
       </c>
       <c r="B70" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C70" s="1">
         <v>44781</v>
@@ -2064,7 +2064,7 @@
         <v>1</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C71" s="1">
         <v>44782</v>
@@ -2081,7 +2081,7 @@
         <v>1</v>
       </c>
       <c r="B72" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C72" s="1">
         <v>44783</v>
@@ -2098,7 +2098,7 @@
         <v>1</v>
       </c>
       <c r="B73" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C73" s="1">
         <v>44784</v>
@@ -2115,7 +2115,7 @@
         <v>1</v>
       </c>
       <c r="B74" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C74" s="1">
         <v>44785</v>
@@ -2132,7 +2132,7 @@
         <v>1</v>
       </c>
       <c r="B75" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C75" s="1">
         <v>44786</v>
@@ -2149,7 +2149,7 @@
         <v>1</v>
       </c>
       <c r="B76" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C76" s="1">
         <v>44787</v>
@@ -2166,7 +2166,7 @@
         <v>1</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C77" s="1">
         <v>44788</v>
@@ -2183,7 +2183,7 @@
         <v>1</v>
       </c>
       <c r="B78" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C78" s="1">
         <v>44789</v>
@@ -2200,7 +2200,7 @@
         <v>1</v>
       </c>
       <c r="B79" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C79" s="1">
         <v>44790</v>
@@ -2217,7 +2217,7 @@
         <v>1</v>
       </c>
       <c r="B80" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C80" s="1">
         <v>44791</v>
@@ -2234,7 +2234,7 @@
         <v>1</v>
       </c>
       <c r="B81" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C81" s="1">
         <v>44792</v>
@@ -2251,7 +2251,7 @@
         <v>1</v>
       </c>
       <c r="B82" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C82" s="1">
         <v>44793</v>
@@ -2268,7 +2268,7 @@
         <v>1</v>
       </c>
       <c r="B83" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C83" s="1">
         <v>44794</v>
@@ -2285,7 +2285,7 @@
         <v>1</v>
       </c>
       <c r="B84" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C84" s="1">
         <v>44795</v>
@@ -2302,7 +2302,7 @@
         <v>1</v>
       </c>
       <c r="B85" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C85" s="1">
         <v>44796</v>
@@ -2319,7 +2319,7 @@
         <v>1</v>
       </c>
       <c r="B86" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C86" s="1">
         <v>44797</v>
@@ -2336,7 +2336,7 @@
         <v>1</v>
       </c>
       <c r="B87" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C87" s="1">
         <v>44798</v>
@@ -2353,7 +2353,7 @@
         <v>1</v>
       </c>
       <c r="B88" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C88" s="1">
         <v>44799</v>
@@ -2370,7 +2370,7 @@
         <v>1</v>
       </c>
       <c r="B89" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C89" s="1">
         <v>44800</v>
@@ -2387,7 +2387,7 @@
         <v>1</v>
       </c>
       <c r="B90" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C90" s="1">
         <v>44801</v>
@@ -2404,7 +2404,7 @@
         <v>1</v>
       </c>
       <c r="B91" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C91" s="1">
         <v>44802</v>
@@ -2421,7 +2421,7 @@
         <v>1</v>
       </c>
       <c r="B92" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C92" s="1">
         <v>44803</v>
@@ -2438,7 +2438,7 @@
         <v>1</v>
       </c>
       <c r="B93" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C93" s="1">
         <v>44804</v>
@@ -2455,7 +2455,7 @@
         <v>1</v>
       </c>
       <c r="B94" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C94" s="1">
         <v>44805</v>
@@ -2472,7 +2472,7 @@
         <v>1</v>
       </c>
       <c r="B95" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C95" s="1">
         <v>44806</v>
@@ -2489,7 +2489,7 @@
         <v>1</v>
       </c>
       <c r="B96" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C96" s="1">
         <v>44807</v>
@@ -2506,7 +2506,7 @@
         <v>1</v>
       </c>
       <c r="B97" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C97" s="1">
         <v>44808</v>
@@ -2523,7 +2523,7 @@
         <v>1</v>
       </c>
       <c r="B98" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C98" s="1">
         <v>44809</v>
@@ -2540,7 +2540,7 @@
         <v>1</v>
       </c>
       <c r="B99" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C99" s="1">
         <v>44810</v>
@@ -2557,7 +2557,7 @@
         <v>1</v>
       </c>
       <c r="B100" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C100" s="1">
         <v>44811</v>
@@ -2574,7 +2574,7 @@
         <v>1</v>
       </c>
       <c r="B101" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C101" s="1">
         <v>44812</v>
@@ -2591,7 +2591,7 @@
         <v>2</v>
       </c>
       <c r="B102" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C102" s="1">
         <v>44713</v>
@@ -2608,7 +2608,7 @@
         <v>2</v>
       </c>
       <c r="B103" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C103" s="1">
         <v>44714</v>
@@ -2625,7 +2625,7 @@
         <v>2</v>
       </c>
       <c r="B104" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C104" s="1">
         <v>44715</v>
@@ -2642,7 +2642,7 @@
         <v>2</v>
       </c>
       <c r="B105" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C105" s="1">
         <v>44716</v>
@@ -2659,7 +2659,7 @@
         <v>2</v>
       </c>
       <c r="B106" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C106" s="1">
         <v>44717</v>
@@ -2676,7 +2676,7 @@
         <v>2</v>
       </c>
       <c r="B107" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C107" s="1">
         <v>44718</v>
@@ -2693,7 +2693,7 @@
         <v>2</v>
       </c>
       <c r="B108" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C108" s="1">
         <v>44719</v>
@@ -2710,7 +2710,7 @@
         <v>2</v>
       </c>
       <c r="B109" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C109" s="1">
         <v>44720</v>
@@ -2727,7 +2727,7 @@
         <v>2</v>
       </c>
       <c r="B110" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C110" s="1">
         <v>44721</v>
@@ -2744,7 +2744,7 @@
         <v>2</v>
       </c>
       <c r="B111" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C111" s="1">
         <v>44722</v>
@@ -2761,7 +2761,7 @@
         <v>2</v>
       </c>
       <c r="B112" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C112" s="1">
         <v>44723</v>
@@ -2778,7 +2778,7 @@
         <v>2</v>
       </c>
       <c r="B113" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C113" s="1">
         <v>44724</v>
@@ -2795,7 +2795,7 @@
         <v>2</v>
       </c>
       <c r="B114" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C114" s="1">
         <v>44725</v>
@@ -2812,7 +2812,7 @@
         <v>2</v>
       </c>
       <c r="B115" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C115" s="1">
         <v>44726</v>
@@ -2829,7 +2829,7 @@
         <v>2</v>
       </c>
       <c r="B116" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C116" s="1">
         <v>44727</v>
@@ -2846,7 +2846,7 @@
         <v>2</v>
       </c>
       <c r="B117" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C117" s="1">
         <v>44728</v>
@@ -2863,7 +2863,7 @@
         <v>2</v>
       </c>
       <c r="B118" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C118" s="1">
         <v>44729</v>
@@ -2880,7 +2880,7 @@
         <v>2</v>
       </c>
       <c r="B119" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C119" s="1">
         <v>44730</v>
@@ -2897,7 +2897,7 @@
         <v>2</v>
       </c>
       <c r="B120" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C120" s="1">
         <v>44731</v>
@@ -2914,7 +2914,7 @@
         <v>2</v>
       </c>
       <c r="B121" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C121" s="1">
         <v>44732</v>
@@ -2931,7 +2931,7 @@
         <v>2</v>
       </c>
       <c r="B122" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C122" s="1">
         <v>44733</v>
@@ -2948,7 +2948,7 @@
         <v>2</v>
       </c>
       <c r="B123" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C123" s="1">
         <v>44734</v>
@@ -2965,7 +2965,7 @@
         <v>2</v>
       </c>
       <c r="B124" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C124" s="1">
         <v>44735</v>
@@ -2982,7 +2982,7 @@
         <v>2</v>
       </c>
       <c r="B125" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C125" s="1">
         <v>44736</v>
@@ -2999,7 +2999,7 @@
         <v>2</v>
       </c>
       <c r="B126" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C126" s="1">
         <v>44737</v>
@@ -3016,7 +3016,7 @@
         <v>2</v>
       </c>
       <c r="B127" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C127" s="1">
         <v>44738</v>
@@ -3033,7 +3033,7 @@
         <v>2</v>
       </c>
       <c r="B128" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C128" s="1">
         <v>44739</v>
@@ -3050,7 +3050,7 @@
         <v>2</v>
       </c>
       <c r="B129" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C129" s="1">
         <v>44740</v>
@@ -3067,7 +3067,7 @@
         <v>2</v>
       </c>
       <c r="B130" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C130" s="1">
         <v>44741</v>
@@ -3084,7 +3084,7 @@
         <v>2</v>
       </c>
       <c r="B131" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C131" s="1">
         <v>44742</v>
@@ -3101,7 +3101,7 @@
         <v>2</v>
       </c>
       <c r="B132" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C132" s="1">
         <v>44743</v>
@@ -3118,7 +3118,7 @@
         <v>2</v>
       </c>
       <c r="B133" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C133" s="1">
         <v>44744</v>
@@ -3135,7 +3135,7 @@
         <v>2</v>
       </c>
       <c r="B134" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C134" s="1">
         <v>44745</v>
@@ -3152,7 +3152,7 @@
         <v>2</v>
       </c>
       <c r="B135" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C135" s="1">
         <v>44746</v>
@@ -3169,7 +3169,7 @@
         <v>2</v>
       </c>
       <c r="B136" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C136" s="1">
         <v>44747</v>
@@ -3186,7 +3186,7 @@
         <v>2</v>
       </c>
       <c r="B137" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C137" s="1">
         <v>44748</v>
@@ -3203,7 +3203,7 @@
         <v>2</v>
       </c>
       <c r="B138" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C138" s="1">
         <v>44749</v>
@@ -3220,7 +3220,7 @@
         <v>2</v>
       </c>
       <c r="B139" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C139" s="1">
         <v>44750</v>
@@ -3237,7 +3237,7 @@
         <v>2</v>
       </c>
       <c r="B140" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C140" s="1">
         <v>44751</v>
@@ -3254,7 +3254,7 @@
         <v>2</v>
       </c>
       <c r="B141" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C141" s="1">
         <v>44752</v>
@@ -3271,7 +3271,7 @@
         <v>2</v>
       </c>
       <c r="B142" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C142" s="1">
         <v>44753</v>
@@ -3288,7 +3288,7 @@
         <v>2</v>
       </c>
       <c r="B143" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C143" s="1">
         <v>44754</v>
@@ -3305,7 +3305,7 @@
         <v>2</v>
       </c>
       <c r="B144" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C144" s="1">
         <v>44755</v>
@@ -3322,7 +3322,7 @@
         <v>2</v>
       </c>
       <c r="B145" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C145" s="1">
         <v>44756</v>
@@ -3339,7 +3339,7 @@
         <v>2</v>
       </c>
       <c r="B146" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C146" s="1">
         <v>44757</v>
@@ -3356,7 +3356,7 @@
         <v>2</v>
       </c>
       <c r="B147" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C147" s="1">
         <v>44758</v>
@@ -3373,7 +3373,7 @@
         <v>2</v>
       </c>
       <c r="B148" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C148" s="1">
         <v>44759</v>
@@ -3390,7 +3390,7 @@
         <v>2</v>
       </c>
       <c r="B149" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C149" s="1">
         <v>44760</v>
@@ -3407,7 +3407,7 @@
         <v>2</v>
       </c>
       <c r="B150" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C150" s="1">
         <v>44761</v>
@@ -3424,7 +3424,7 @@
         <v>2</v>
       </c>
       <c r="B151" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C151" s="1">
         <v>44762</v>
@@ -3441,7 +3441,7 @@
         <v>2</v>
       </c>
       <c r="B152" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C152" s="1">
         <v>44763</v>
@@ -3458,7 +3458,7 @@
         <v>2</v>
       </c>
       <c r="B153" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C153" s="1">
         <v>44764</v>
@@ -3475,7 +3475,7 @@
         <v>2</v>
       </c>
       <c r="B154" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C154" s="1">
         <v>44765</v>
@@ -3492,7 +3492,7 @@
         <v>2</v>
       </c>
       <c r="B155" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C155" s="1">
         <v>44766</v>
@@ -3509,7 +3509,7 @@
         <v>2</v>
       </c>
       <c r="B156" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C156" s="1">
         <v>44767</v>
@@ -3526,7 +3526,7 @@
         <v>2</v>
       </c>
       <c r="B157" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C157" s="1">
         <v>44768</v>
@@ -3543,7 +3543,7 @@
         <v>2</v>
       </c>
       <c r="B158" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C158" s="1">
         <v>44769</v>
@@ -3560,7 +3560,7 @@
         <v>2</v>
       </c>
       <c r="B159" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C159" s="1">
         <v>44770</v>
@@ -3577,7 +3577,7 @@
         <v>2</v>
       </c>
       <c r="B160" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C160" s="1">
         <v>44771</v>
@@ -3594,7 +3594,7 @@
         <v>2</v>
       </c>
       <c r="B161" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C161" s="1">
         <v>44772</v>
@@ -3611,7 +3611,7 @@
         <v>2</v>
       </c>
       <c r="B162" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C162" s="1">
         <v>44773</v>
@@ -3628,7 +3628,7 @@
         <v>2</v>
       </c>
       <c r="B163" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C163" s="1">
         <v>44774</v>
@@ -3645,7 +3645,7 @@
         <v>2</v>
       </c>
       <c r="B164" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C164" s="1">
         <v>44775</v>
@@ -3662,7 +3662,7 @@
         <v>2</v>
       </c>
       <c r="B165" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C165" s="1">
         <v>44776</v>
@@ -3679,7 +3679,7 @@
         <v>2</v>
       </c>
       <c r="B166" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C166" s="1">
         <v>44777</v>
@@ -3696,7 +3696,7 @@
         <v>2</v>
       </c>
       <c r="B167" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C167" s="1">
         <v>44778</v>
@@ -3713,7 +3713,7 @@
         <v>2</v>
       </c>
       <c r="B168" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C168" s="1">
         <v>44779</v>
@@ -3730,7 +3730,7 @@
         <v>2</v>
       </c>
       <c r="B169" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C169" s="1">
         <v>44780</v>
@@ -3747,7 +3747,7 @@
         <v>2</v>
       </c>
       <c r="B170" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C170" s="1">
         <v>44781</v>
@@ -3764,7 +3764,7 @@
         <v>2</v>
       </c>
       <c r="B171" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C171" s="1">
         <v>44782</v>
@@ -3781,7 +3781,7 @@
         <v>2</v>
       </c>
       <c r="B172" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C172" s="1">
         <v>44783</v>
@@ -3798,7 +3798,7 @@
         <v>2</v>
       </c>
       <c r="B173" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C173" s="1">
         <v>44784</v>
@@ -3815,7 +3815,7 @@
         <v>2</v>
       </c>
       <c r="B174" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C174" s="1">
         <v>44785</v>
@@ -3832,7 +3832,7 @@
         <v>2</v>
       </c>
       <c r="B175" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C175" s="1">
         <v>44786</v>
@@ -3849,7 +3849,7 @@
         <v>2</v>
       </c>
       <c r="B176" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C176" s="1">
         <v>44787</v>
@@ -3866,7 +3866,7 @@
         <v>2</v>
       </c>
       <c r="B177" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C177" s="1">
         <v>44788</v>
@@ -3883,7 +3883,7 @@
         <v>2</v>
       </c>
       <c r="B178" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C178" s="1">
         <v>44789</v>
@@ -3900,7 +3900,7 @@
         <v>2</v>
       </c>
       <c r="B179" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C179" s="1">
         <v>44790</v>
@@ -3917,7 +3917,7 @@
         <v>2</v>
       </c>
       <c r="B180" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C180" s="1">
         <v>44791</v>
@@ -3934,7 +3934,7 @@
         <v>2</v>
       </c>
       <c r="B181" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C181" s="1">
         <v>44792</v>
@@ -3951,7 +3951,7 @@
         <v>2</v>
       </c>
       <c r="B182" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C182" s="1">
         <v>44793</v>
@@ -3968,7 +3968,7 @@
         <v>2</v>
       </c>
       <c r="B183" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C183" s="1">
         <v>44794</v>
@@ -3985,7 +3985,7 @@
         <v>2</v>
       </c>
       <c r="B184" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C184" s="1">
         <v>44795</v>
@@ -4002,7 +4002,7 @@
         <v>2</v>
       </c>
       <c r="B185" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C185" s="1">
         <v>44796</v>
@@ -4019,7 +4019,7 @@
         <v>2</v>
       </c>
       <c r="B186" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C186" s="1">
         <v>44797</v>
@@ -4036,7 +4036,7 @@
         <v>2</v>
       </c>
       <c r="B187" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C187" s="1">
         <v>44798</v>
@@ -4053,7 +4053,7 @@
         <v>2</v>
       </c>
       <c r="B188" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C188" s="1">
         <v>44799</v>
@@ -4070,7 +4070,7 @@
         <v>2</v>
       </c>
       <c r="B189" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C189" s="1">
         <v>44800</v>
@@ -4087,7 +4087,7 @@
         <v>2</v>
       </c>
       <c r="B190" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C190" s="1">
         <v>44801</v>
@@ -4104,7 +4104,7 @@
         <v>2</v>
       </c>
       <c r="B191" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C191" s="1">
         <v>44802</v>
@@ -4121,7 +4121,7 @@
         <v>2</v>
       </c>
       <c r="B192" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C192" s="1">
         <v>44803</v>
@@ -4138,7 +4138,7 @@
         <v>2</v>
       </c>
       <c r="B193" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C193" s="1">
         <v>44804</v>
@@ -4155,7 +4155,7 @@
         <v>2</v>
       </c>
       <c r="B194" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C194" s="1">
         <v>44805</v>
@@ -4172,7 +4172,7 @@
         <v>2</v>
       </c>
       <c r="B195" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C195" s="1">
         <v>44806</v>
@@ -4189,7 +4189,7 @@
         <v>2</v>
       </c>
       <c r="B196" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C196" s="1">
         <v>44807</v>
@@ -4206,7 +4206,7 @@
         <v>2</v>
       </c>
       <c r="B197" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C197" s="1">
         <v>44808</v>
@@ -4223,7 +4223,7 @@
         <v>2</v>
       </c>
       <c r="B198" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C198" s="1">
         <v>44809</v>
@@ -4240,7 +4240,7 @@
         <v>2</v>
       </c>
       <c r="B199" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C199" s="1">
         <v>44810</v>
@@ -4257,7 +4257,7 @@
         <v>2</v>
       </c>
       <c r="B200" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C200" s="1">
         <v>44811</v>
@@ -4274,7 +4274,7 @@
         <v>2</v>
       </c>
       <c r="B201" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C201" s="1">
         <v>44812</v>
@@ -4291,7 +4291,7 @@
         <v>3</v>
       </c>
       <c r="B202" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C202" s="1">
         <v>44713</v>
@@ -4308,7 +4308,7 @@
         <v>3</v>
       </c>
       <c r="B203" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C203" s="1">
         <v>44714</v>
@@ -4325,7 +4325,7 @@
         <v>3</v>
       </c>
       <c r="B204" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C204" s="1">
         <v>44715</v>
@@ -4342,7 +4342,7 @@
         <v>3</v>
       </c>
       <c r="B205" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C205" s="1">
         <v>44716</v>
@@ -4359,7 +4359,7 @@
         <v>3</v>
       </c>
       <c r="B206" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C206" s="1">
         <v>44717</v>
@@ -4376,7 +4376,7 @@
         <v>3</v>
       </c>
       <c r="B207" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C207" s="1">
         <v>44718</v>
@@ -4393,7 +4393,7 @@
         <v>3</v>
       </c>
       <c r="B208" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C208" s="1">
         <v>44719</v>
@@ -4410,7 +4410,7 @@
         <v>3</v>
       </c>
       <c r="B209" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C209" s="1">
         <v>44720</v>
@@ -4427,7 +4427,7 @@
         <v>3</v>
       </c>
       <c r="B210" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C210" s="1">
         <v>44721</v>
@@ -4444,7 +4444,7 @@
         <v>3</v>
       </c>
       <c r="B211" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C211" s="1">
         <v>44722</v>
@@ -4461,7 +4461,7 @@
         <v>3</v>
       </c>
       <c r="B212" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C212" s="1">
         <v>44723</v>
@@ -4478,7 +4478,7 @@
         <v>3</v>
       </c>
       <c r="B213" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C213" s="1">
         <v>44724</v>
@@ -4495,7 +4495,7 @@
         <v>3</v>
       </c>
       <c r="B214" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C214" s="1">
         <v>44725</v>
@@ -4512,7 +4512,7 @@
         <v>3</v>
       </c>
       <c r="B215" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C215" s="1">
         <v>44726</v>
@@ -4529,7 +4529,7 @@
         <v>3</v>
       </c>
       <c r="B216" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C216" s="1">
         <v>44727</v>
@@ -4546,7 +4546,7 @@
         <v>3</v>
       </c>
       <c r="B217" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C217" s="1">
         <v>44728</v>
@@ -4563,7 +4563,7 @@
         <v>3</v>
       </c>
       <c r="B218" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C218" s="1">
         <v>44729</v>
@@ -4580,7 +4580,7 @@
         <v>3</v>
       </c>
       <c r="B219" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C219" s="1">
         <v>44730</v>
@@ -4597,7 +4597,7 @@
         <v>3</v>
       </c>
       <c r="B220" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C220" s="1">
         <v>44731</v>
@@ -4614,7 +4614,7 @@
         <v>3</v>
       </c>
       <c r="B221" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C221" s="1">
         <v>44732</v>
@@ -4631,7 +4631,7 @@
         <v>3</v>
       </c>
       <c r="B222" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C222" s="1">
         <v>44733</v>
@@ -4648,7 +4648,7 @@
         <v>3</v>
       </c>
       <c r="B223" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C223" s="1">
         <v>44734</v>
@@ -4665,7 +4665,7 @@
         <v>3</v>
       </c>
       <c r="B224" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C224" s="1">
         <v>44735</v>
@@ -4682,7 +4682,7 @@
         <v>3</v>
       </c>
       <c r="B225" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C225" s="1">
         <v>44736</v>
@@ -4699,7 +4699,7 @@
         <v>3</v>
       </c>
       <c r="B226" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C226" s="1">
         <v>44737</v>
@@ -4716,7 +4716,7 @@
         <v>3</v>
       </c>
       <c r="B227" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C227" s="1">
         <v>44738</v>
@@ -4733,7 +4733,7 @@
         <v>3</v>
       </c>
       <c r="B228" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C228" s="1">
         <v>44739</v>
@@ -4750,7 +4750,7 @@
         <v>3</v>
       </c>
       <c r="B229" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C229" s="1">
         <v>44740</v>
@@ -4767,7 +4767,7 @@
         <v>3</v>
       </c>
       <c r="B230" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C230" s="1">
         <v>44741</v>
@@ -4784,7 +4784,7 @@
         <v>3</v>
       </c>
       <c r="B231" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C231" s="1">
         <v>44742</v>
@@ -4801,7 +4801,7 @@
         <v>3</v>
       </c>
       <c r="B232" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C232" s="1">
         <v>44743</v>
@@ -4818,7 +4818,7 @@
         <v>3</v>
       </c>
       <c r="B233" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C233" s="1">
         <v>44744</v>
@@ -4835,7 +4835,7 @@
         <v>3</v>
       </c>
       <c r="B234" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C234" s="1">
         <v>44745</v>
@@ -4852,7 +4852,7 @@
         <v>3</v>
       </c>
       <c r="B235" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C235" s="1">
         <v>44746</v>
@@ -4869,7 +4869,7 @@
         <v>3</v>
       </c>
       <c r="B236" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C236" s="1">
         <v>44747</v>
@@ -4886,7 +4886,7 @@
         <v>3</v>
       </c>
       <c r="B237" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C237" s="1">
         <v>44748</v>
@@ -4903,7 +4903,7 @@
         <v>3</v>
       </c>
       <c r="B238" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C238" s="1">
         <v>44749</v>
@@ -4920,7 +4920,7 @@
         <v>3</v>
       </c>
       <c r="B239" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C239" s="1">
         <v>44750</v>
@@ -4937,7 +4937,7 @@
         <v>3</v>
       </c>
       <c r="B240" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C240" s="1">
         <v>44751</v>
@@ -4954,7 +4954,7 @@
         <v>3</v>
       </c>
       <c r="B241" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C241" s="1">
         <v>44752</v>
@@ -4971,7 +4971,7 @@
         <v>3</v>
       </c>
       <c r="B242" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C242" s="1">
         <v>44753</v>
@@ -4988,7 +4988,7 @@
         <v>3</v>
       </c>
       <c r="B243" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C243" s="1">
         <v>44754</v>
@@ -5005,7 +5005,7 @@
         <v>3</v>
       </c>
       <c r="B244" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C244" s="1">
         <v>44755</v>
@@ -5022,7 +5022,7 @@
         <v>3</v>
       </c>
       <c r="B245" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C245" s="1">
         <v>44756</v>
@@ -5039,7 +5039,7 @@
         <v>3</v>
       </c>
       <c r="B246" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C246" s="1">
         <v>44757</v>
@@ -5056,7 +5056,7 @@
         <v>3</v>
       </c>
       <c r="B247" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C247" s="1">
         <v>44758</v>
@@ -5073,7 +5073,7 @@
         <v>3</v>
       </c>
       <c r="B248" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C248" s="1">
         <v>44759</v>
@@ -5090,7 +5090,7 @@
         <v>3</v>
       </c>
       <c r="B249" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C249" s="1">
         <v>44760</v>
@@ -5107,7 +5107,7 @@
         <v>3</v>
       </c>
       <c r="B250" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C250" s="1">
         <v>44761</v>
@@ -5124,7 +5124,7 @@
         <v>3</v>
       </c>
       <c r="B251" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C251" s="1">
         <v>44762</v>
@@ -5141,7 +5141,7 @@
         <v>3</v>
       </c>
       <c r="B252" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C252" s="1">
         <v>44763</v>
@@ -5158,7 +5158,7 @@
         <v>3</v>
       </c>
       <c r="B253" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C253" s="1">
         <v>44764</v>
@@ -5175,7 +5175,7 @@
         <v>3</v>
       </c>
       <c r="B254" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C254" s="1">
         <v>44765</v>
@@ -5192,7 +5192,7 @@
         <v>3</v>
       </c>
       <c r="B255" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C255" s="1">
         <v>44766</v>
@@ -5209,7 +5209,7 @@
         <v>3</v>
       </c>
       <c r="B256" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C256" s="1">
         <v>44767</v>
@@ -5226,7 +5226,7 @@
         <v>3</v>
       </c>
       <c r="B257" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C257" s="1">
         <v>44768</v>
@@ -5243,7 +5243,7 @@
         <v>3</v>
       </c>
       <c r="B258" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C258" s="1">
         <v>44769</v>
@@ -5260,7 +5260,7 @@
         <v>3</v>
       </c>
       <c r="B259" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C259" s="1">
         <v>44770</v>
@@ -5277,7 +5277,7 @@
         <v>3</v>
       </c>
       <c r="B260" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C260" s="1">
         <v>44771</v>
@@ -5294,7 +5294,7 @@
         <v>3</v>
       </c>
       <c r="B261" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C261" s="1">
         <v>44772</v>
@@ -5311,7 +5311,7 @@
         <v>3</v>
       </c>
       <c r="B262" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C262" s="1">
         <v>44773</v>
@@ -5328,7 +5328,7 @@
         <v>3</v>
       </c>
       <c r="B263" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C263" s="1">
         <v>44774</v>
@@ -5345,7 +5345,7 @@
         <v>3</v>
       </c>
       <c r="B264" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C264" s="1">
         <v>44775</v>
@@ -5362,7 +5362,7 @@
         <v>3</v>
       </c>
       <c r="B265" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C265" s="1">
         <v>44776</v>
@@ -5379,7 +5379,7 @@
         <v>3</v>
       </c>
       <c r="B266" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C266" s="1">
         <v>44777</v>
@@ -5396,7 +5396,7 @@
         <v>3</v>
       </c>
       <c r="B267" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C267" s="1">
         <v>44778</v>
@@ -5413,7 +5413,7 @@
         <v>3</v>
       </c>
       <c r="B268" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C268" s="1">
         <v>44779</v>
@@ -5430,7 +5430,7 @@
         <v>3</v>
       </c>
       <c r="B269" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C269" s="1">
         <v>44780</v>
@@ -5447,7 +5447,7 @@
         <v>3</v>
       </c>
       <c r="B270" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C270" s="1">
         <v>44781</v>
@@ -5464,7 +5464,7 @@
         <v>3</v>
       </c>
       <c r="B271" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C271" s="1">
         <v>44782</v>
@@ -5481,7 +5481,7 @@
         <v>3</v>
       </c>
       <c r="B272" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C272" s="1">
         <v>44783</v>
@@ -5498,7 +5498,7 @@
         <v>3</v>
       </c>
       <c r="B273" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C273" s="1">
         <v>44784</v>
@@ -5515,7 +5515,7 @@
         <v>3</v>
       </c>
       <c r="B274" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C274" s="1">
         <v>44785</v>
@@ -5532,7 +5532,7 @@
         <v>3</v>
       </c>
       <c r="B275" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C275" s="1">
         <v>44786</v>
@@ -5549,7 +5549,7 @@
         <v>3</v>
       </c>
       <c r="B276" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C276" s="1">
         <v>44787</v>
@@ -5566,7 +5566,7 @@
         <v>3</v>
       </c>
       <c r="B277" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C277" s="1">
         <v>44788</v>
@@ -5583,7 +5583,7 @@
         <v>3</v>
       </c>
       <c r="B278" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C278" s="1">
         <v>44789</v>
@@ -5600,7 +5600,7 @@
         <v>3</v>
       </c>
       <c r="B279" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C279" s="1">
         <v>44790</v>
@@ -5617,7 +5617,7 @@
         <v>3</v>
       </c>
       <c r="B280" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C280" s="1">
         <v>44791</v>
@@ -5634,7 +5634,7 @@
         <v>3</v>
       </c>
       <c r="B281" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C281" s="1">
         <v>44792</v>
@@ -5651,7 +5651,7 @@
         <v>3</v>
       </c>
       <c r="B282" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C282" s="1">
         <v>44793</v>
@@ -5668,7 +5668,7 @@
         <v>3</v>
       </c>
       <c r="B283" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C283" s="1">
         <v>44794</v>
@@ -5685,7 +5685,7 @@
         <v>3</v>
       </c>
       <c r="B284" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C284" s="1">
         <v>44795</v>
@@ -5702,7 +5702,7 @@
         <v>3</v>
       </c>
       <c r="B285" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C285" s="1">
         <v>44796</v>
@@ -5719,7 +5719,7 @@
         <v>3</v>
       </c>
       <c r="B286" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C286" s="1">
         <v>44797</v>
@@ -5736,7 +5736,7 @@
         <v>3</v>
       </c>
       <c r="B287" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C287" s="1">
         <v>44798</v>
@@ -5753,7 +5753,7 @@
         <v>3</v>
       </c>
       <c r="B288" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C288" s="1">
         <v>44799</v>
@@ -5770,7 +5770,7 @@
         <v>3</v>
       </c>
       <c r="B289" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C289" s="1">
         <v>44800</v>
@@ -5787,7 +5787,7 @@
         <v>3</v>
       </c>
       <c r="B290" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C290" s="1">
         <v>44801</v>
@@ -5804,7 +5804,7 @@
         <v>3</v>
       </c>
       <c r="B291" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C291" s="1">
         <v>44802</v>
@@ -5821,7 +5821,7 @@
         <v>3</v>
       </c>
       <c r="B292" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C292" s="1">
         <v>44803</v>
@@ -5838,7 +5838,7 @@
         <v>3</v>
       </c>
       <c r="B293" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C293" s="1">
         <v>44804</v>
@@ -5855,7 +5855,7 @@
         <v>3</v>
       </c>
       <c r="B294" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C294" s="1">
         <v>44805</v>
@@ -5872,7 +5872,7 @@
         <v>3</v>
       </c>
       <c r="B295" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C295" s="1">
         <v>44806</v>
@@ -5889,7 +5889,7 @@
         <v>3</v>
       </c>
       <c r="B296" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C296" s="1">
         <v>44807</v>
@@ -5906,7 +5906,7 @@
         <v>3</v>
       </c>
       <c r="B297" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C297" s="1">
         <v>44808</v>
@@ -5923,7 +5923,7 @@
         <v>3</v>
       </c>
       <c r="B298" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C298" s="1">
         <v>44809</v>
@@ -5940,7 +5940,7 @@
         <v>3</v>
       </c>
       <c r="B299" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C299" s="1">
         <v>44810</v>
@@ -5957,7 +5957,7 @@
         <v>3</v>
       </c>
       <c r="B300" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C300" s="1">
         <v>44811</v>
@@ -5974,7 +5974,7 @@
         <v>3</v>
       </c>
       <c r="B301" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C301" s="1">
         <v>44812</v>

</xml_diff>